<commit_message>
ExcelTotalsPanel can work with parent data context now. Also aggregation function results can be passed as method parameter.
</commit_message>
<xml_diff>
--- a/ExcelReportGenerator.Tests/TestData/TotalsPanelRenderTest/TestPanelRender.xlsx
+++ b/ExcelReportGenerator.Tests/TestData/TotalsPanelRenderTest/TestPanelRender.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <x:si>
     <x:t>Changed plain text</x:t>
   </x:si>
@@ -22,10 +22,16 @@
     <x:t>930,708</x:t>
   </x:si>
   <x:si>
-    <x:t>Text1 3 Text2 1888,86 Text3 5500,80</x:t>
+    <x:t>Text1 3 Text2 1888,86 String parameter 5500,80 5500,80</x:t>
   </x:si>
   <x:si>
     <x:t>{Mix(di:Sum)}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>55,8000</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Aggregation: 7389,66. Date: 25.10.2017</x:t>
   </x:si>
   <x:si>
     <x:t>{Sum(di:Sum)}</x:t>
@@ -379,13 +385,13 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:I1"/>
+  <x:dimension ref="A1:M1"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:9">
+    <x:row r="1" spans="1:13">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -410,8 +416,20 @@
       <x:c r="H1" s="0">
         <x:f>ROW()</x:f>
       </x:c>
-      <x:c r="I1" s="0" t="s">
+      <x:c r="I1" s="0" t="n">
+        <x:v>20171025</x:v>
+      </x:c>
+      <x:c r="J1" s="0" t="n">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="K1" s="0" t="s">
         <x:v>4</x:v>
+      </x:c>
+      <x:c r="L1" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="M1" s="0" t="s">
+        <x:v>6</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>